<commit_message>
[fix]: fix capital letters in subject
</commit_message>
<xml_diff>
--- a/src/extraResources/2022.xlsx
+++ b/src/extraResources/2022.xlsx
@@ -290,9 +290,6 @@
     <t>Моделирование и прототипирование</t>
   </si>
   <si>
-    <t>информационная безопасность</t>
-  </si>
-  <si>
     <t>Робототехника</t>
   </si>
   <si>
@@ -546,6 +543,9 @@
   </si>
   <si>
     <t>Количество учебных недель</t>
+  </si>
+  <si>
+    <t>Информационная безопасность</t>
   </si>
 </sst>
 </file>
@@ -1016,45 +1016,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1068,13 +1029,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1082,15 +1037,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1098,9 +1044,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1114,16 +1057,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1143,6 +1080,69 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1445,7 +1445,7 @@
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D1" s="53"/>
       <c r="E1" s="53"/>
@@ -1465,16 +1465,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
@@ -1523,14 +1523,14 @@
       <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
-        <v>122</v>
+      <c r="A6" s="110" t="s">
+        <v>121</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -1540,12 +1540,12 @@
       <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A7" s="81"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -1555,14 +1555,14 @@
       <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
-        <v>124</v>
+      <c r="A8" s="110" t="s">
+        <v>123</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -1572,12 +1572,12 @@
       <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -1611,7 +1611,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -1622,13 +1622,13 @@
     </row>
     <row r="12" spans="1:64" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>128</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -1638,14 +1638,14 @@
       <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="81" t="s">
-        <v>129</v>
+      <c r="A13" s="110" t="s">
+        <v>128</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1655,9 +1655,9 @@
       <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
+      <c r="A14" s="110"/>
       <c r="B14" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
@@ -1668,9 +1668,9 @@
       <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
@@ -1681,9 +1681,9 @@
       <c r="I15" s="27"/>
     </row>
     <row r="16" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="81"/>
+      <c r="A16" s="110"/>
       <c r="B16" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
@@ -1749,9 +1749,9 @@
       <c r="BL16" s="65"/>
     </row>
     <row r="17" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="81"/>
+      <c r="A17" s="110"/>
       <c r="B17" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
@@ -1817,9 +1817,9 @@
       <c r="BL17" s="65"/>
     </row>
     <row r="18" spans="1:64" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="81"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
@@ -1885,9 +1885,9 @@
       <c r="BL18" s="65"/>
     </row>
     <row r="19" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="81"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
@@ -1953,14 +1953,14 @@
       <c r="BL19" s="65"/>
     </row>
     <row r="20" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="110" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>106</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -2025,12 +2025,12 @@
       <c r="BL20" s="65"/>
     </row>
     <row r="21" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A21" s="81"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -2096,13 +2096,13 @@
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -2174,7 +2174,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B27" s="44"/>
       <c r="C27" s="11"/>
@@ -2507,13 +2507,13 @@
       <c r="BL27" s="65"/>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A28" s="106" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="112" t="s">
-        <v>160</v>
-      </c>
-      <c r="C28" s="118"/>
+      <c r="A28" s="91" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="99"/>
       <c r="D28" s="44"/>
       <c r="E28" s="44"/>
       <c r="F28" s="44"/>
@@ -2577,16 +2577,16 @@
       <c r="BL28" s="65"/>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="111" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="122" t="s">
+      <c r="C29" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="123" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="117"/>
+      <c r="D29" s="98"/>
       <c r="E29" s="76"/>
       <c r="F29" s="76"/>
       <c r="G29" s="44"/>
@@ -2649,15 +2649,15 @@
       <c r="BL29" s="65"/>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A30" s="124"/>
-      <c r="B30" s="129">
+      <c r="A30" s="112"/>
+      <c r="B30" s="108">
         <v>2954</v>
       </c>
-      <c r="C30" s="130">
+      <c r="C30" s="109">
         <v>3190</v>
       </c>
-      <c r="D30" s="119"/>
-      <c r="E30" s="120"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="101"/>
       <c r="F30" s="76"/>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
@@ -2719,22 +2719,22 @@
       <c r="BL30" s="65"/>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A31" s="101" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="125">
-        <v>1</v>
-      </c>
-      <c r="C31" s="125">
+      <c r="A31" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="104">
+        <v>1</v>
+      </c>
+      <c r="C31" s="104">
         <v>2</v>
       </c>
-      <c r="D31" s="125">
+      <c r="D31" s="104">
         <v>3</v>
       </c>
-      <c r="E31" s="126">
+      <c r="E31" s="105">
         <v>4</v>
       </c>
-      <c r="F31" s="94"/>
+      <c r="F31" s="81"/>
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
       <c r="I31" s="73"/>
@@ -2795,20 +2795,20 @@
       <c r="BL31" s="65"/>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A32" s="103"/>
-      <c r="B32" s="127">
+      <c r="A32" s="114"/>
+      <c r="B32" s="106">
         <v>21</v>
       </c>
-      <c r="C32" s="127">
+      <c r="C32" s="106">
         <v>23</v>
       </c>
-      <c r="D32" s="127">
+      <c r="D32" s="106">
         <v>23</v>
       </c>
-      <c r="E32" s="128">
+      <c r="E32" s="107">
         <v>23</v>
       </c>
-      <c r="F32" s="95"/>
+      <c r="F32" s="82"/>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
       <c r="I32" s="73"/>
@@ -2869,22 +2869,22 @@
       <c r="BL32" s="65"/>
     </row>
     <row r="33" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A33" s="101" t="s">
-        <v>172</v>
-      </c>
-      <c r="B33" s="125">
-        <v>1</v>
-      </c>
-      <c r="C33" s="125">
+      <c r="A33" s="113" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="104">
+        <v>1</v>
+      </c>
+      <c r="C33" s="104">
         <v>2</v>
       </c>
-      <c r="D33" s="125">
+      <c r="D33" s="104">
         <v>3</v>
       </c>
-      <c r="E33" s="126">
+      <c r="E33" s="105">
         <v>4</v>
       </c>
-      <c r="F33" s="94"/>
+      <c r="F33" s="81"/>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
       <c r="I33" s="73"/>
@@ -2945,20 +2945,20 @@
       <c r="BL33" s="65"/>
     </row>
     <row r="34" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A34" s="103"/>
-      <c r="B34" s="127">
+      <c r="A34" s="114"/>
+      <c r="B34" s="106">
         <v>33</v>
       </c>
-      <c r="C34" s="127">
+      <c r="C34" s="106">
         <v>34</v>
       </c>
-      <c r="D34" s="127">
+      <c r="D34" s="106">
         <v>34</v>
       </c>
-      <c r="E34" s="128">
+      <c r="E34" s="107">
         <v>34</v>
       </c>
-      <c r="F34" s="95"/>
+      <c r="F34" s="82"/>
       <c r="G34" s="44"/>
       <c r="H34" s="44"/>
       <c r="I34" s="73"/>
@@ -3020,14 +3020,14 @@
     </row>
     <row r="35" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A35" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="B35" s="99" t="s">
-        <v>165</v>
-      </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="115"/>
-      <c r="E35" s="100"/>
+      <c r="C35" s="87"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="87"/>
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
       <c r="H35" s="44"/>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="37" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B37" s="77"/>
       <c r="C37" s="44"/>
@@ -3224,7 +3224,7 @@
     </row>
     <row r="38" spans="1:64" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B38" s="44"/>
       <c r="C38" s="44"/>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="39" spans="1:64" s="69" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B39" s="44"/>
       <c r="C39" s="44"/>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="40" spans="1:64" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" s="44"/>
       <c r="C40" s="44"/>
@@ -3537,7 +3537,7 @@
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D1" s="53"/>
       <c r="E1" s="53"/>
@@ -3576,73 +3576,73 @@
         <v>5</v>
       </c>
       <c r="D2" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="L2" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="M2" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>157</v>
-      </c>
       <c r="O2" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="R2" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="S2" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="T2" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="U2" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="V2" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="W2" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="X2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="Y2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="Z2" s="28" t="s">
         <v>95</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y2" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z2" s="28" t="s">
-        <v>96</v>
       </c>
       <c r="AA2" s="44"/>
       <c r="AB2" s="44"/>
@@ -3786,14 +3786,14 @@
       <c r="AB5" s="44"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="110" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -3828,12 +3828,12 @@
       <c r="AB6" s="44"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="81"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -3862,14 +3862,14 @@
       <c r="AB7" s="44"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="110" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -3898,12 +3898,12 @@
       <c r="AB8" s="44"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -3932,14 +3932,14 @@
       <c r="AB9" s="44"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="110" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -3974,12 +3974,12 @@
       <c r="AB10" s="44"/>
     </row>
     <row r="11" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="81"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -4014,14 +4014,14 @@
       <c r="AB11" s="44"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="110" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -4050,24 +4050,24 @@
       <c r="V12" s="45"/>
       <c r="W12" s="45"/>
       <c r="X12" s="57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y12" s="57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z12" s="57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA12" s="44"/>
       <c r="AB12" s="44"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A13" s="81"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -4102,14 +4102,14 @@
       <c r="AB13" s="44"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="110" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -4138,12 +4138,12 @@
       <c r="AB14" s="44"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -4172,12 +4172,12 @@
       <c r="AB15" s="44"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A16" s="81"/>
+      <c r="A16" s="110"/>
       <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
@@ -4206,14 +4206,14 @@
       <c r="AB16" s="44"/>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A17" s="81" t="s">
-        <v>101</v>
+      <c r="A17" s="110" t="s">
+        <v>100</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -4242,12 +4242,12 @@
       <c r="AB17" s="44"/>
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A18" s="81"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -4282,12 +4282,12 @@
       <c r="AB18" s="44"/>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A19" s="81"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -4323,13 +4323,13 @@
     </row>
     <row r="20" spans="1:64" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -4358,14 +4358,14 @@
       <c r="AB20" s="44"/>
     </row>
     <row r="21" spans="1:64" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="110" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -4394,12 +4394,12 @@
       <c r="AB21" s="44"/>
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A22" s="81"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -4429,13 +4429,13 @@
     </row>
     <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -4470,14 +4470,14 @@
       <c r="AB23" s="44"/>
     </row>
     <row r="24" spans="1:64" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="81" t="s">
-        <v>109</v>
+      <c r="A24" s="110" t="s">
+        <v>108</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -4506,12 +4506,12 @@
       <c r="AB24" s="44"/>
     </row>
     <row r="25" spans="1:64" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="81"/>
+      <c r="A25" s="110"/>
       <c r="B25" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
@@ -4602,10 +4602,10 @@
       <c r="AB27" s="44"/>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A28" s="83" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="83"/>
+      <c r="A28" s="115" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="115"/>
       <c r="C28" s="58"/>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
@@ -4615,10 +4615,10 @@
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
-      <c r="L28" s="82">
+      <c r="L28" s="117">
         <v>2</v>
       </c>
-      <c r="M28" s="82"/>
+      <c r="M28" s="117"/>
       <c r="N28" s="45"/>
       <c r="O28" s="45"/>
       <c r="P28" s="45"/>
@@ -4636,10 +4636,10 @@
       <c r="AB28" s="44"/>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A29" s="83" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="83"/>
+      <c r="A29" s="115" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="115"/>
       <c r="C29" s="58"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
@@ -4650,10 +4650,10 @@
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
-      <c r="M29" s="82">
+      <c r="M29" s="117">
         <v>2</v>
       </c>
-      <c r="N29" s="82"/>
+      <c r="N29" s="117"/>
       <c r="O29" s="45"/>
       <c r="P29" s="45"/>
       <c r="Q29" s="45"/>
@@ -4670,10 +4670,10 @@
       <c r="AB29" s="44"/>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A30" s="83" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="83"/>
+      <c r="A30" s="115" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="115"/>
       <c r="C30" s="58"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -4684,10 +4684,10 @@
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
-      <c r="M30" s="82">
+      <c r="M30" s="117">
         <v>2</v>
       </c>
-      <c r="N30" s="82"/>
+      <c r="N30" s="117"/>
       <c r="O30" s="45"/>
       <c r="P30" s="45"/>
       <c r="Q30" s="45"/>
@@ -4704,10 +4704,10 @@
       <c r="AB30" s="44"/>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A31" s="83" t="s">
+      <c r="A31" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="83"/>
+      <c r="B31" s="115"/>
       <c r="C31" s="58"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -4742,10 +4742,10 @@
       <c r="AB31" s="44"/>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A32" s="83" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32" s="83"/>
+      <c r="A32" s="115" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="115"/>
       <c r="C32" s="58"/>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -4761,11 +4761,11 @@
       <c r="O32" s="45"/>
       <c r="P32" s="45"/>
       <c r="Q32" s="45"/>
-      <c r="R32" s="84">
+      <c r="R32" s="116">
         <v>2</v>
       </c>
-      <c r="S32" s="84"/>
-      <c r="T32" s="84"/>
+      <c r="S32" s="116"/>
+      <c r="T32" s="116"/>
       <c r="U32" s="45"/>
       <c r="V32" s="45"/>
       <c r="W32" s="45"/>
@@ -4812,10 +4812,10 @@
       <c r="BL32" s="61"/>
     </row>
     <row r="33" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A33" s="83" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="83"/>
+      <c r="A33" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="115"/>
       <c r="C33" s="58"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -4831,11 +4831,11 @@
       <c r="O33" s="45"/>
       <c r="P33" s="45"/>
       <c r="Q33" s="45"/>
-      <c r="R33" s="84">
+      <c r="R33" s="116">
         <v>2</v>
       </c>
-      <c r="S33" s="84"/>
-      <c r="T33" s="84"/>
+      <c r="S33" s="116"/>
+      <c r="T33" s="116"/>
       <c r="U33" s="45"/>
       <c r="V33" s="45"/>
       <c r="W33" s="45"/>
@@ -4882,10 +4882,10 @@
       <c r="BL33" s="61"/>
     </row>
     <row r="34" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A34" s="83" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="83"/>
+      <c r="A34" s="115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="115"/>
       <c r="C34" s="58"/>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -4904,10 +4904,10 @@
       <c r="R34" s="45"/>
       <c r="S34" s="45"/>
       <c r="T34" s="45"/>
-      <c r="U34" s="84">
+      <c r="U34" s="116">
         <v>2</v>
       </c>
-      <c r="V34" s="84"/>
+      <c r="V34" s="116"/>
       <c r="W34" s="45"/>
       <c r="X34" s="45"/>
       <c r="Y34" s="45"/>
@@ -4952,10 +4952,10 @@
       <c r="BL34" s="61"/>
     </row>
     <row r="35" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A35" s="83" t="s">
-        <v>116</v>
-      </c>
-      <c r="B35" s="83"/>
+      <c r="A35" s="115" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="115"/>
       <c r="C35" s="58"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -4975,10 +4975,10 @@
       <c r="S35" s="45"/>
       <c r="T35" s="45"/>
       <c r="U35" s="45"/>
-      <c r="V35" s="84">
+      <c r="V35" s="116">
         <v>2</v>
       </c>
-      <c r="W35" s="84"/>
+      <c r="W35" s="116"/>
       <c r="X35" s="45"/>
       <c r="Y35" s="45"/>
       <c r="Z35" s="45"/>
@@ -5089,7 +5089,7 @@
     </row>
     <row r="37" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B37" s="44"/>
       <c r="C37" s="44"/>
@@ -5156,13 +5156,13 @@
       <c r="BL37" s="61"/>
     </row>
     <row r="38" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A38" s="106" t="s">
-        <v>171</v>
-      </c>
-      <c r="B38" s="112" t="s">
-        <v>161</v>
-      </c>
-      <c r="C38" s="108"/>
+      <c r="A38" s="91" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" s="94" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="93"/>
       <c r="D38" s="44"/>
       <c r="E38" s="44"/>
       <c r="F38" s="44"/>
@@ -5226,16 +5226,16 @@
       <c r="BL38" s="61"/>
     </row>
     <row r="39" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A39" s="110" t="s">
+      <c r="A39" s="118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="102" t="s">
+      <c r="C39" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="96" t="s">
-        <v>121</v>
-      </c>
-      <c r="D39" s="105"/>
+      <c r="D39" s="90"/>
       <c r="E39" s="44"/>
       <c r="F39" s="44"/>
       <c r="G39" s="44"/>
@@ -5298,16 +5298,16 @@
       <c r="BL39" s="61"/>
     </row>
     <row r="40" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A40" s="116"/>
+      <c r="A40" s="119"/>
       <c r="B40" s="72">
         <v>5058</v>
       </c>
-      <c r="C40" s="98">
+      <c r="C40" s="85">
         <v>5549</v>
       </c>
-      <c r="D40" s="114"/>
-      <c r="E40" s="108"/>
-      <c r="F40" s="108"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="93"/>
       <c r="G40" s="44"/>
       <c r="H40" s="44"/>
       <c r="I40" s="44"/>
@@ -5368,25 +5368,25 @@
       <c r="BL40" s="61"/>
     </row>
     <row r="41" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A41" s="101" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" s="102">
+      <c r="A41" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="88">
         <v>5</v>
       </c>
-      <c r="C41" s="102">
+      <c r="C41" s="88">
         <v>6</v>
       </c>
-      <c r="D41" s="102">
+      <c r="D41" s="88">
         <v>7</v>
       </c>
-      <c r="E41" s="102">
+      <c r="E41" s="88">
         <v>8</v>
       </c>
-      <c r="F41" s="96">
+      <c r="F41" s="83">
         <v>9</v>
       </c>
-      <c r="G41" s="113"/>
+      <c r="G41" s="95"/>
       <c r="H41" s="44"/>
       <c r="I41" s="44"/>
       <c r="J41" s="44"/>
@@ -5446,23 +5446,23 @@
       <c r="BL41" s="61"/>
     </row>
     <row r="42" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A42" s="103"/>
-      <c r="B42" s="104">
+      <c r="A42" s="114"/>
+      <c r="B42" s="89">
         <v>29</v>
       </c>
-      <c r="C42" s="104">
+      <c r="C42" s="89">
         <v>30</v>
       </c>
-      <c r="D42" s="104">
+      <c r="D42" s="89">
         <v>32</v>
       </c>
-      <c r="E42" s="104">
+      <c r="E42" s="89">
         <v>33</v>
       </c>
-      <c r="F42" s="97">
+      <c r="F42" s="84">
         <v>33</v>
       </c>
-      <c r="G42" s="105"/>
+      <c r="G42" s="90"/>
       <c r="H42" s="44"/>
       <c r="I42" s="44"/>
       <c r="J42" s="44"/>
@@ -5522,25 +5522,25 @@
       <c r="BL42" s="61"/>
     </row>
     <row r="43" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A43" s="101" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" s="102">
+      <c r="A43" s="113" t="s">
+        <v>171</v>
+      </c>
+      <c r="B43" s="88">
         <v>5</v>
       </c>
-      <c r="C43" s="102">
+      <c r="C43" s="88">
         <v>6</v>
       </c>
-      <c r="D43" s="102">
+      <c r="D43" s="88">
         <v>7</v>
       </c>
-      <c r="E43" s="102">
+      <c r="E43" s="88">
         <v>8</v>
       </c>
-      <c r="F43" s="96">
+      <c r="F43" s="83">
         <v>9</v>
       </c>
-      <c r="G43" s="113"/>
+      <c r="G43" s="95"/>
       <c r="H43" s="44"/>
       <c r="I43" s="44"/>
       <c r="J43" s="44"/>
@@ -5600,23 +5600,23 @@
       <c r="BL43" s="61"/>
     </row>
     <row r="44" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A44" s="103"/>
-      <c r="B44" s="104">
+      <c r="A44" s="114"/>
+      <c r="B44" s="89">
         <v>34</v>
       </c>
-      <c r="C44" s="104">
+      <c r="C44" s="89">
         <v>34</v>
       </c>
-      <c r="D44" s="104">
+      <c r="D44" s="89">
         <v>34</v>
       </c>
-      <c r="E44" s="104">
+      <c r="E44" s="89">
         <v>34</v>
       </c>
-      <c r="F44" s="97">
+      <c r="F44" s="84">
         <v>33</v>
       </c>
-      <c r="G44" s="105"/>
+      <c r="G44" s="90"/>
       <c r="H44" s="44"/>
       <c r="I44" s="44"/>
       <c r="J44" s="44"/>
@@ -5677,15 +5677,15 @@
     </row>
     <row r="45" spans="1:64" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="B45" s="99" t="s">
-        <v>165</v>
-      </c>
-      <c r="C45" s="100"/>
-      <c r="D45" s="115"/>
-      <c r="E45" s="100"/>
-      <c r="F45" s="100"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="97"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
       <c r="G45" s="44"/>
       <c r="H45" s="44"/>
       <c r="I45" s="44"/>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="47" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="44"/>
       <c r="C47" s="44"/>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="48" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A48" s="50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" s="44"/>
       <c r="C48" s="44"/>
@@ -5949,7 +5949,7 @@
     </row>
     <row r="49" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="44"/>
       <c r="C49" s="44"/>
@@ -5981,7 +5981,7 @@
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B50" s="44"/>
       <c r="C50" s="44"/>
@@ -6107,6 +6107,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="A33:B33"/>
@@ -6120,19 +6133,6 @@
     <mergeCell ref="R32:T32"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A34:B34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6143,8 +6143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="59" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U73" sqref="U73"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="59" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="V52" sqref="V52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6170,127 +6170,127 @@
       <c r="A1" s="27"/>
       <c r="B1" s="27"/>
       <c r="C1" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="89" t="s">
-        <v>155</v>
-      </c>
-      <c r="O1" s="89"/>
+        <v>158</v>
+      </c>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="122" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="122"/>
       <c r="P1" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="X1" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AD1" s="122" t="s">
         <v>147</v>
       </c>
-      <c r="AC1" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD1" s="89" t="s">
+      <c r="AE1" s="122"/>
+      <c r="AF1" s="122" t="s">
         <v>148</v>
       </c>
-      <c r="AE1" s="89"/>
-      <c r="AF1" s="89" t="s">
+      <c r="AG1" s="122"/>
+      <c r="AH1" s="122" t="s">
         <v>149</v>
       </c>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="89" t="s">
+      <c r="AI1" s="122"/>
+      <c r="AJ1" s="122" t="s">
         <v>150</v>
       </c>
-      <c r="AI1" s="89"/>
-      <c r="AJ1" s="89" t="s">
+      <c r="AK1" s="122"/>
+      <c r="AL1" s="122" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM1" s="122"/>
+      <c r="AN1" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="AK1" s="89"/>
-      <c r="AL1" s="89" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM1" s="89"/>
-      <c r="AN1" s="89" t="s">
+      <c r="AO1" s="122"/>
+      <c r="AP1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ1" s="122"/>
+      <c r="AR1" s="122" t="s">
         <v>152</v>
       </c>
-      <c r="AO1" s="89"/>
-      <c r="AP1" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ1" s="89"/>
-      <c r="AR1" s="89" t="s">
+      <c r="AS1" s="122"/>
+      <c r="AT1" s="122" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU1" s="122"/>
+      <c r="AV1" s="122" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW1" s="122"/>
+      <c r="AX1" s="122" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY1" s="122"/>
+      <c r="AZ1" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="BA1" s="122"/>
+      <c r="BB1" s="122" t="s">
         <v>153</v>
       </c>
-      <c r="AS1" s="89"/>
-      <c r="AT1" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="AU1" s="89"/>
-      <c r="AV1" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW1" s="89"/>
-      <c r="AX1" s="89" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY1" s="89"/>
-      <c r="AZ1" s="89" t="s">
-        <v>152</v>
-      </c>
-      <c r="BA1" s="89"/>
-      <c r="BB1" s="89" t="s">
+      <c r="BC1" s="122"/>
+      <c r="BD1" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="BC1" s="89"/>
-      <c r="BD1" s="28" t="s">
-        <v>155</v>
-      </c>
       <c r="BE1" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BF1" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BG1" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BH1" s="27"/>
       <c r="BI1" s="27"/>
@@ -6312,130 +6312,130 @@
         <v>6</v>
       </c>
       <c r="F2" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="I2" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="J2" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="K2" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="L2" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="M2" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>92</v>
-      </c>
       <c r="N2" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="Q2" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="R2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="AE2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="AF2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="AG2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="AH2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="AI2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="AK2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="X2" s="28" t="s">
+      <c r="AL2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="AM2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="Z2" s="28" t="s">
+      <c r="AN2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="AA2" s="28" t="s">
+      <c r="AO2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="AB2" s="28" t="s">
+      <c r="AP2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="AC2" s="28" t="s">
+      <c r="AQ2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="AD2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AG2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AH2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AI2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AM2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AN2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AO2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP2" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="AQ2" s="28" t="s">
-        <v>138</v>
-      </c>
       <c r="AR2" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AS2" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AT2" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AU2" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AV2" s="28" t="s">
         <v>7</v>
@@ -6450,22 +6450,22 @@
         <v>7</v>
       </c>
       <c r="AZ2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="BA2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="BB2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="BC2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="BD2" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="BA2" s="28" t="s">
+      <c r="BE2" s="31" t="s">
         <v>139</v>
-      </c>
-      <c r="BB2" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="BC2" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="BD2" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="BE2" s="31" t="s">
-        <v>140</v>
       </c>
       <c r="BF2" s="31" t="s">
         <v>8</v>
@@ -6780,7 +6780,7 @@
       <c r="BI5" s="27"/>
     </row>
     <row r="6" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="110" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -6865,7 +6865,7 @@
       <c r="BI6" s="27"/>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A7" s="81"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
@@ -6944,7 +6944,7 @@
       <c r="BI7" s="27"/>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="110" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -7013,7 +7013,7 @@
       <c r="BI8" s="27"/>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -7080,7 +7080,7 @@
       <c r="BI9" s="27"/>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="110" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -7165,7 +7165,7 @@
       <c r="BI10" s="27"/>
     </row>
     <row r="11" spans="1:61" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="81"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
@@ -7232,7 +7232,7 @@
       <c r="BI11" s="27"/>
     </row>
     <row r="12" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="110" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -7241,194 +7241,194 @@
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="85">
-        <v>1</v>
-      </c>
-      <c r="E12" s="86"/>
-      <c r="F12" s="85">
-        <v>1</v>
-      </c>
-      <c r="G12" s="86"/>
-      <c r="H12" s="85">
-        <v>1</v>
-      </c>
-      <c r="I12" s="86"/>
-      <c r="J12" s="85">
-        <v>1</v>
-      </c>
-      <c r="K12" s="86"/>
-      <c r="L12" s="85">
-        <v>1</v>
-      </c>
-      <c r="M12" s="86"/>
-      <c r="N12" s="85">
-        <v>1</v>
-      </c>
-      <c r="O12" s="86"/>
-      <c r="P12" s="85">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="85">
-        <v>1</v>
-      </c>
-      <c r="S12" s="86"/>
-      <c r="T12" s="85">
-        <v>1</v>
-      </c>
-      <c r="U12" s="86"/>
-      <c r="V12" s="85">
-        <v>1</v>
-      </c>
-      <c r="W12" s="86"/>
-      <c r="X12" s="85">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="86"/>
-      <c r="Z12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="86"/>
-      <c r="AB12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="86"/>
-      <c r="AD12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="86"/>
-      <c r="AF12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="86"/>
-      <c r="AH12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="86"/>
-      <c r="AJ12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AK12" s="86"/>
-      <c r="AL12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="86"/>
+      <c r="D12" s="127">
+        <v>1</v>
+      </c>
+      <c r="E12" s="128"/>
+      <c r="F12" s="127">
+        <v>1</v>
+      </c>
+      <c r="G12" s="128"/>
+      <c r="H12" s="127">
+        <v>1</v>
+      </c>
+      <c r="I12" s="128"/>
+      <c r="J12" s="127">
+        <v>1</v>
+      </c>
+      <c r="K12" s="128"/>
+      <c r="L12" s="127">
+        <v>1</v>
+      </c>
+      <c r="M12" s="128"/>
+      <c r="N12" s="127">
+        <v>1</v>
+      </c>
+      <c r="O12" s="128"/>
+      <c r="P12" s="127">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="128"/>
+      <c r="R12" s="127">
+        <v>1</v>
+      </c>
+      <c r="S12" s="128"/>
+      <c r="T12" s="127">
+        <v>1</v>
+      </c>
+      <c r="U12" s="128"/>
+      <c r="V12" s="127">
+        <v>1</v>
+      </c>
+      <c r="W12" s="128"/>
+      <c r="X12" s="127">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="128"/>
+      <c r="Z12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="128"/>
+      <c r="AB12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="128"/>
+      <c r="AD12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="128"/>
+      <c r="AF12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="128"/>
+      <c r="AH12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="128"/>
+      <c r="AJ12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="128"/>
+      <c r="AL12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="128"/>
       <c r="AN12" s="40">
         <v>1</v>
       </c>
       <c r="AO12" s="40">
         <v>1</v>
       </c>
-      <c r="AP12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AQ12" s="86"/>
-      <c r="AR12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AS12" s="86"/>
-      <c r="AT12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AU12" s="86"/>
-      <c r="AV12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AW12" s="86"/>
-      <c r="AX12" s="85">
-        <v>1</v>
-      </c>
-      <c r="AY12" s="86"/>
+      <c r="AP12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="128"/>
+      <c r="AR12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="128"/>
+      <c r="AT12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AU12" s="128"/>
+      <c r="AV12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="128"/>
+      <c r="AX12" s="127">
+        <v>1</v>
+      </c>
+      <c r="AY12" s="128"/>
       <c r="AZ12" s="40">
         <v>1</v>
       </c>
       <c r="BA12" s="40">
         <v>1</v>
       </c>
-      <c r="BB12" s="85">
-        <v>1</v>
-      </c>
-      <c r="BC12" s="86"/>
-      <c r="BD12" s="85">
-        <v>1</v>
-      </c>
-      <c r="BE12" s="86"/>
-      <c r="BF12" s="85">
-        <v>1</v>
-      </c>
-      <c r="BG12" s="86"/>
+      <c r="BB12" s="127">
+        <v>1</v>
+      </c>
+      <c r="BC12" s="128"/>
+      <c r="BD12" s="127">
+        <v>1</v>
+      </c>
+      <c r="BE12" s="128"/>
+      <c r="BF12" s="127">
+        <v>1</v>
+      </c>
+      <c r="BG12" s="128"/>
       <c r="BH12" s="27"/>
       <c r="BI12" s="27"/>
     </row>
     <row r="13" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="81"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="88"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="88"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="88"/>
-      <c r="R13" s="87"/>
-      <c r="S13" s="88"/>
-      <c r="T13" s="87"/>
-      <c r="U13" s="88"/>
-      <c r="V13" s="87"/>
-      <c r="W13" s="88"/>
-      <c r="X13" s="87"/>
-      <c r="Y13" s="88"/>
-      <c r="Z13" s="87"/>
-      <c r="AA13" s="88"/>
-      <c r="AB13" s="87"/>
-      <c r="AC13" s="88"/>
-      <c r="AD13" s="87"/>
-      <c r="AE13" s="88"/>
-      <c r="AF13" s="87"/>
-      <c r="AG13" s="88"/>
-      <c r="AH13" s="87"/>
-      <c r="AI13" s="88"/>
-      <c r="AJ13" s="87"/>
-      <c r="AK13" s="88"/>
-      <c r="AL13" s="87"/>
-      <c r="AM13" s="88"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="130"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="130"/>
+      <c r="N13" s="129"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="129"/>
+      <c r="Q13" s="130"/>
+      <c r="R13" s="129"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="129"/>
+      <c r="U13" s="130"/>
+      <c r="V13" s="129"/>
+      <c r="W13" s="130"/>
+      <c r="X13" s="129"/>
+      <c r="Y13" s="130"/>
+      <c r="Z13" s="129"/>
+      <c r="AA13" s="130"/>
+      <c r="AB13" s="129"/>
+      <c r="AC13" s="130"/>
+      <c r="AD13" s="129"/>
+      <c r="AE13" s="130"/>
+      <c r="AF13" s="129"/>
+      <c r="AG13" s="130"/>
+      <c r="AH13" s="129"/>
+      <c r="AI13" s="130"/>
+      <c r="AJ13" s="129"/>
+      <c r="AK13" s="130"/>
+      <c r="AL13" s="129"/>
+      <c r="AM13" s="130"/>
       <c r="AN13" s="33"/>
       <c r="AO13" s="33"/>
-      <c r="AP13" s="87"/>
-      <c r="AQ13" s="88"/>
-      <c r="AR13" s="87"/>
-      <c r="AS13" s="88"/>
-      <c r="AT13" s="87"/>
-      <c r="AU13" s="88"/>
-      <c r="AV13" s="87"/>
-      <c r="AW13" s="88"/>
-      <c r="AX13" s="87"/>
-      <c r="AY13" s="88"/>
+      <c r="AP13" s="129"/>
+      <c r="AQ13" s="130"/>
+      <c r="AR13" s="129"/>
+      <c r="AS13" s="130"/>
+      <c r="AT13" s="129"/>
+      <c r="AU13" s="130"/>
+      <c r="AV13" s="129"/>
+      <c r="AW13" s="130"/>
+      <c r="AX13" s="129"/>
+      <c r="AY13" s="130"/>
       <c r="AZ13" s="33"/>
       <c r="BA13" s="33"/>
-      <c r="BB13" s="87"/>
-      <c r="BC13" s="88"/>
-      <c r="BD13" s="87"/>
-      <c r="BE13" s="88"/>
-      <c r="BF13" s="87"/>
-      <c r="BG13" s="88"/>
+      <c r="BB13" s="129"/>
+      <c r="BC13" s="130"/>
+      <c r="BD13" s="129"/>
+      <c r="BE13" s="130"/>
+      <c r="BF13" s="129"/>
+      <c r="BG13" s="130"/>
       <c r="BH13" s="27"/>
       <c r="BI13" s="27"/>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
+      <c r="A14" s="110"/>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
@@ -7503,7 +7503,7 @@
       <c r="BI14" s="27"/>
     </row>
     <row r="15" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
@@ -7574,7 +7574,7 @@
       <c r="BI15" s="27"/>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A16" s="81"/>
+      <c r="A16" s="110"/>
       <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
@@ -7645,7 +7645,7 @@
       <c r="BI16" s="27"/>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A17" s="81"/>
+      <c r="A17" s="110"/>
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
@@ -7712,7 +7712,7 @@
       <c r="BI17" s="27"/>
     </row>
     <row r="18" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="110" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -7843,7 +7843,7 @@
       <c r="BI18" s="27"/>
     </row>
     <row r="19" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="81"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="2" t="s">
         <v>31</v>
       </c>
@@ -7942,7 +7942,7 @@
       <c r="BI19" s="27"/>
     </row>
     <row r="20" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="110" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -8057,7 +8057,7 @@
       <c r="BI20" s="27"/>
     </row>
     <row r="21" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A21" s="81"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -8146,7 +8146,7 @@
       <c r="BI21" s="27"/>
     </row>
     <row r="22" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="81"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -8234,7 +8234,7 @@
       <c r="BI22" s="27"/>
     </row>
     <row r="23" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="81"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="6" t="s">
         <v>38</v>
       </c>
@@ -8301,7 +8301,7 @@
       <c r="BI23" s="27"/>
     </row>
     <row r="24" spans="1:61" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="110" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -8370,7 +8370,7 @@
       <c r="BI24" s="27"/>
     </row>
     <row r="25" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="81"/>
+      <c r="A25" s="110"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
@@ -8437,7 +8437,7 @@
       <c r="BI25" s="27"/>
     </row>
     <row r="26" spans="1:61" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="81"/>
+      <c r="A26" s="110"/>
       <c r="B26" s="6" t="s">
         <v>42</v>
       </c>
@@ -8504,10 +8504,10 @@
       <c r="BI26" s="27"/>
     </row>
     <row r="27" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="93"/>
+      <c r="B27" s="125"/>
       <c r="C27" s="17"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -8697,10 +8697,10 @@
       <c r="BI29" s="27"/>
     </row>
     <row r="30" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="124" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="91"/>
+      <c r="B30" s="124"/>
       <c r="C30" s="18"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -8712,10 +8712,10 @@
       <c r="K30" s="33"/>
       <c r="L30" s="33"/>
       <c r="M30" s="33"/>
-      <c r="N30" s="90">
+      <c r="N30" s="126">
         <v>2</v>
       </c>
-      <c r="O30" s="90"/>
+      <c r="O30" s="126"/>
       <c r="P30" s="33"/>
       <c r="Q30" s="33"/>
       <c r="R30" s="33"/>
@@ -8764,10 +8764,10 @@
       <c r="BI30" s="27"/>
     </row>
     <row r="31" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A31" s="91" t="s">
+      <c r="A31" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="91"/>
+      <c r="B31" s="124"/>
       <c r="C31" s="18"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -8831,10 +8831,10 @@
       <c r="BI31" s="27"/>
     </row>
     <row r="32" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A32" s="91" t="s">
+      <c r="A32" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="91"/>
+      <c r="B32" s="124"/>
       <c r="C32" s="18"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -8848,10 +8848,10 @@
       <c r="M32" s="33"/>
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
-      <c r="P32" s="90">
+      <c r="P32" s="126">
         <v>2</v>
       </c>
-      <c r="Q32" s="90"/>
+      <c r="Q32" s="126"/>
       <c r="R32" s="42"/>
       <c r="S32" s="42"/>
       <c r="T32" s="42"/>
@@ -8898,10 +8898,10 @@
       <c r="BI32" s="27"/>
     </row>
     <row r="33" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="91" t="s">
+      <c r="A33" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="91"/>
+      <c r="B33" s="124"/>
       <c r="C33" s="18"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -8915,10 +8915,10 @@
       <c r="M33" s="33"/>
       <c r="N33" s="33"/>
       <c r="O33" s="33"/>
-      <c r="P33" s="90">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="90"/>
+      <c r="P33" s="126">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="126"/>
       <c r="R33" s="42"/>
       <c r="S33" s="42"/>
       <c r="T33" s="42"/>
@@ -8965,10 +8965,10 @@
       <c r="BI33" s="27"/>
     </row>
     <row r="34" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="91" t="s">
+      <c r="A34" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="91"/>
+      <c r="B34" s="124"/>
       <c r="C34" s="18"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -8984,10 +8984,10 @@
       <c r="O34" s="33"/>
       <c r="P34" s="42"/>
       <c r="Q34" s="42"/>
-      <c r="R34" s="90">
-        <v>1</v>
-      </c>
-      <c r="S34" s="90"/>
+      <c r="R34" s="126">
+        <v>1</v>
+      </c>
+      <c r="S34" s="126"/>
       <c r="T34" s="42"/>
       <c r="U34" s="42"/>
       <c r="V34" s="33"/>
@@ -9032,10 +9032,10 @@
       <c r="BI34" s="27"/>
     </row>
     <row r="35" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="91" t="s">
+      <c r="A35" s="124" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="91"/>
+      <c r="B35" s="124"/>
       <c r="C35" s="18"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -9051,10 +9051,10 @@
       <c r="O35" s="33"/>
       <c r="P35" s="42"/>
       <c r="Q35" s="42"/>
-      <c r="R35" s="90">
+      <c r="R35" s="126">
         <v>2</v>
       </c>
-      <c r="S35" s="90"/>
+      <c r="S35" s="126"/>
       <c r="T35" s="42"/>
       <c r="U35" s="42"/>
       <c r="V35" s="33"/>
@@ -9099,10 +9099,10 @@
       <c r="BI35" s="27"/>
     </row>
     <row r="36" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="91" t="s">
+      <c r="A36" s="124" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="91"/>
+      <c r="B36" s="124"/>
       <c r="C36" s="18"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -9120,10 +9120,10 @@
       <c r="Q36" s="42"/>
       <c r="R36" s="33"/>
       <c r="S36" s="33"/>
-      <c r="T36" s="90">
+      <c r="T36" s="126">
         <v>2</v>
       </c>
-      <c r="U36" s="90"/>
+      <c r="U36" s="126"/>
       <c r="V36" s="33"/>
       <c r="W36" s="33"/>
       <c r="X36" s="33"/>
@@ -9166,10 +9166,10 @@
       <c r="BI36" s="27"/>
     </row>
     <row r="37" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="91" t="s">
+      <c r="A37" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="91"/>
+      <c r="B37" s="124"/>
       <c r="C37" s="18"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -9187,10 +9187,10 @@
       <c r="Q37" s="42"/>
       <c r="R37" s="33"/>
       <c r="S37" s="33"/>
-      <c r="T37" s="90">
+      <c r="T37" s="126">
         <v>2</v>
       </c>
-      <c r="U37" s="90"/>
+      <c r="U37" s="126"/>
       <c r="V37" s="33"/>
       <c r="W37" s="33"/>
       <c r="X37" s="33"/>
@@ -9233,10 +9233,10 @@
       <c r="BI37" s="27"/>
     </row>
     <row r="38" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="91"/>
+      <c r="B38" s="124"/>
       <c r="C38" s="18"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -9256,10 +9256,10 @@
       <c r="S38" s="33"/>
       <c r="T38" s="33"/>
       <c r="U38" s="33"/>
-      <c r="V38" s="90">
+      <c r="V38" s="126">
         <v>2</v>
       </c>
-      <c r="W38" s="90"/>
+      <c r="W38" s="126"/>
       <c r="X38" s="33"/>
       <c r="Y38" s="33"/>
       <c r="Z38" s="33"/>
@@ -9300,10 +9300,10 @@
       <c r="BI38" s="27"/>
     </row>
     <row r="39" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="91"/>
+      <c r="B39" s="124"/>
       <c r="C39" s="18"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -9323,10 +9323,10 @@
       <c r="S39" s="33"/>
       <c r="T39" s="33"/>
       <c r="U39" s="33"/>
-      <c r="V39" s="90">
+      <c r="V39" s="126">
         <v>2</v>
       </c>
-      <c r="W39" s="90"/>
+      <c r="W39" s="126"/>
       <c r="X39" s="33"/>
       <c r="Y39" s="33"/>
       <c r="Z39" s="33"/>
@@ -9367,10 +9367,10 @@
       <c r="BI39" s="27"/>
     </row>
     <row r="40" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A40" s="91" t="s">
+      <c r="A40" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="91"/>
+      <c r="B40" s="124"/>
       <c r="C40" s="18"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -9392,10 +9392,10 @@
       <c r="U40" s="33"/>
       <c r="V40" s="33"/>
       <c r="W40" s="33"/>
-      <c r="X40" s="90">
+      <c r="X40" s="126">
         <v>2</v>
       </c>
-      <c r="Y40" s="90"/>
+      <c r="Y40" s="126"/>
       <c r="Z40" s="33"/>
       <c r="AA40" s="33"/>
       <c r="AB40" s="33"/>
@@ -9434,10 +9434,10 @@
       <c r="BI40" s="27"/>
     </row>
     <row r="41" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A41" s="91" t="s">
+      <c r="A41" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="91"/>
+      <c r="B41" s="124"/>
       <c r="C41" s="18"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -9459,10 +9459,10 @@
       <c r="U41" s="33"/>
       <c r="V41" s="33"/>
       <c r="W41" s="33"/>
-      <c r="X41" s="90">
+      <c r="X41" s="126">
         <v>2</v>
       </c>
-      <c r="Y41" s="90"/>
+      <c r="Y41" s="126"/>
       <c r="Z41" s="33"/>
       <c r="AA41" s="33"/>
       <c r="AB41" s="33"/>
@@ -9501,10 +9501,10 @@
       <c r="BI41" s="27"/>
     </row>
     <row r="42" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A42" s="91" t="s">
+      <c r="A42" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="91"/>
+      <c r="B42" s="124"/>
       <c r="C42" s="18"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -9528,10 +9528,10 @@
       <c r="W42" s="33"/>
       <c r="X42" s="33"/>
       <c r="Y42" s="33"/>
-      <c r="Z42" s="90">
+      <c r="Z42" s="126">
         <v>2</v>
       </c>
-      <c r="AA42" s="90"/>
+      <c r="AA42" s="126"/>
       <c r="AB42" s="33"/>
       <c r="AC42" s="33"/>
       <c r="AD42" s="33"/>
@@ -9568,10 +9568,10 @@
       <c r="BI42" s="27"/>
     </row>
     <row r="43" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A43" s="91" t="s">
+      <c r="A43" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="91"/>
+      <c r="B43" s="124"/>
       <c r="C43" s="18"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -9595,10 +9595,10 @@
       <c r="W43" s="33"/>
       <c r="X43" s="33"/>
       <c r="Y43" s="33"/>
-      <c r="Z43" s="90">
+      <c r="Z43" s="126">
         <v>2</v>
       </c>
-      <c r="AA43" s="90"/>
+      <c r="AA43" s="126"/>
       <c r="AB43" s="33"/>
       <c r="AC43" s="33"/>
       <c r="AD43" s="33"/>
@@ -9635,10 +9635,10 @@
       <c r="BI43" s="27"/>
     </row>
     <row r="44" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A44" s="91" t="s">
+      <c r="A44" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="91"/>
+      <c r="B44" s="124"/>
       <c r="C44" s="18"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -9688,14 +9688,14 @@
       <c r="AW44" s="33"/>
       <c r="AX44" s="33"/>
       <c r="AY44" s="33"/>
-      <c r="AZ44" s="90">
+      <c r="AZ44" s="126">
         <v>2</v>
       </c>
-      <c r="BA44" s="90"/>
-      <c r="BB44" s="90">
+      <c r="BA44" s="126"/>
+      <c r="BB44" s="126">
         <v>2</v>
       </c>
-      <c r="BC44" s="90"/>
+      <c r="BC44" s="126"/>
       <c r="BD44" s="33"/>
       <c r="BE44" s="33"/>
       <c r="BF44" s="33"/>
@@ -9704,10 +9704,10 @@
       <c r="BI44" s="27"/>
     </row>
     <row r="45" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A45" s="91" t="s">
+      <c r="A45" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="91"/>
+      <c r="B45" s="124"/>
       <c r="C45" s="18"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -9757,10 +9757,10 @@
       <c r="AW45" s="33"/>
       <c r="AX45" s="33"/>
       <c r="AY45" s="33"/>
-      <c r="AZ45" s="90">
+      <c r="AZ45" s="126">
         <v>2</v>
       </c>
-      <c r="BA45" s="90"/>
+      <c r="BA45" s="126"/>
       <c r="BB45" s="33"/>
       <c r="BC45" s="33"/>
       <c r="BD45" s="33"/>
@@ -9771,10 +9771,10 @@
       <c r="BI45" s="27"/>
     </row>
     <row r="46" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A46" s="91" t="s">
+      <c r="A46" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="91"/>
+      <c r="B46" s="124"/>
       <c r="C46" s="18"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -9826,10 +9826,10 @@
       <c r="AY46" s="33"/>
       <c r="AZ46" s="33"/>
       <c r="BA46" s="33"/>
-      <c r="BB46" s="90">
+      <c r="BB46" s="126">
         <v>2</v>
       </c>
-      <c r="BC46" s="90"/>
+      <c r="BC46" s="126"/>
       <c r="BD46" s="33"/>
       <c r="BE46" s="33"/>
       <c r="BF46" s="33"/>
@@ -9838,10 +9838,10 @@
       <c r="BI46" s="27"/>
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A47" s="91" t="s">
+      <c r="A47" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="91"/>
+      <c r="B47" s="124"/>
       <c r="C47" s="18"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -9895,20 +9895,20 @@
       <c r="BA47" s="33"/>
       <c r="BB47" s="33"/>
       <c r="BC47" s="33"/>
-      <c r="BD47" s="90">
+      <c r="BD47" s="126">
         <v>2</v>
       </c>
-      <c r="BE47" s="90"/>
+      <c r="BE47" s="126"/>
       <c r="BF47" s="33"/>
       <c r="BG47" s="33"/>
       <c r="BH47" s="27"/>
       <c r="BI47" s="27"/>
     </row>
     <row r="48" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A48" s="91" t="s">
+      <c r="A48" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="91"/>
+      <c r="B48" s="124"/>
       <c r="C48" s="18"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -9962,20 +9962,20 @@
       <c r="BA48" s="33"/>
       <c r="BB48" s="33"/>
       <c r="BC48" s="33"/>
-      <c r="BD48" s="90">
+      <c r="BD48" s="126">
         <v>2</v>
       </c>
-      <c r="BE48" s="90"/>
+      <c r="BE48" s="126"/>
       <c r="BF48" s="33"/>
       <c r="BG48" s="33"/>
       <c r="BH48" s="27"/>
       <c r="BI48" s="27"/>
     </row>
     <row r="49" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A49" s="91" t="s">
+      <c r="A49" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="91"/>
+      <c r="B49" s="124"/>
       <c r="C49" s="18"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -10031,18 +10031,18 @@
       <c r="BC49" s="33"/>
       <c r="BD49" s="33"/>
       <c r="BE49" s="33"/>
-      <c r="BF49" s="90">
+      <c r="BF49" s="126">
         <v>2</v>
       </c>
-      <c r="BG49" s="90"/>
+      <c r="BG49" s="126"/>
       <c r="BH49" s="27"/>
       <c r="BI49" s="27"/>
     </row>
     <row r="50" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A50" s="91" t="s">
+      <c r="A50" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="91"/>
+      <c r="B50" s="124"/>
       <c r="C50" s="18"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -10098,18 +10098,18 @@
       <c r="BC50" s="33"/>
       <c r="BD50" s="33"/>
       <c r="BE50" s="33"/>
-      <c r="BF50" s="90">
+      <c r="BF50" s="126">
         <v>2</v>
       </c>
-      <c r="BG50" s="90"/>
+      <c r="BG50" s="126"/>
       <c r="BH50" s="27"/>
       <c r="BI50" s="27"/>
     </row>
     <row r="51" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A51" s="91" t="s">
+      <c r="A51" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="91"/>
+      <c r="B51" s="124"/>
       <c r="C51" s="18"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -10137,42 +10137,42 @@
       <c r="AA51" s="33"/>
       <c r="AB51" s="33"/>
       <c r="AC51" s="33"/>
-      <c r="AD51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AE51" s="90"/>
-      <c r="AF51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AG51" s="90"/>
-      <c r="AH51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AI51" s="90"/>
-      <c r="AJ51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AK51" s="90"/>
-      <c r="AL51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AM51" s="90"/>
-      <c r="AN51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AO51" s="90"/>
-      <c r="AP51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AQ51" s="90"/>
-      <c r="AR51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AS51" s="90"/>
-      <c r="AT51" s="90">
-        <v>1</v>
-      </c>
-      <c r="AU51" s="90"/>
+      <c r="AD51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AE51" s="126"/>
+      <c r="AF51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="126"/>
+      <c r="AH51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AI51" s="126"/>
+      <c r="AJ51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AK51" s="126"/>
+      <c r="AL51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AM51" s="126"/>
+      <c r="AN51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AO51" s="126"/>
+      <c r="AP51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AQ51" s="126"/>
+      <c r="AR51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AS51" s="126"/>
+      <c r="AT51" s="126">
+        <v>1</v>
+      </c>
+      <c r="AU51" s="126"/>
       <c r="AV51" s="33"/>
       <c r="AW51" s="33"/>
       <c r="AX51" s="33"/>
@@ -10189,10 +10189,10 @@
       <c r="BI51" s="27"/>
     </row>
     <row r="52" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A52" s="91" t="s">
+      <c r="A52" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="91"/>
+      <c r="B52" s="124"/>
       <c r="C52" s="18"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -10226,10 +10226,10 @@
       <c r="AG52" s="33"/>
       <c r="AH52" s="33"/>
       <c r="AI52" s="33"/>
-      <c r="AJ52" s="90">
-        <v>1</v>
-      </c>
-      <c r="AK52" s="90"/>
+      <c r="AJ52" s="126">
+        <v>1</v>
+      </c>
+      <c r="AK52" s="126"/>
       <c r="AL52" s="33"/>
       <c r="AM52" s="33"/>
       <c r="AN52" s="33"/>
@@ -10256,10 +10256,10 @@
       <c r="BI52" s="27"/>
     </row>
     <row r="53" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A53" s="91" t="s">
+      <c r="A53" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="91"/>
+      <c r="B53" s="124"/>
       <c r="C53" s="18"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -10285,10 +10285,10 @@
       <c r="Y53" s="33"/>
       <c r="Z53" s="33"/>
       <c r="AA53" s="33"/>
-      <c r="AB53" s="90">
+      <c r="AB53" s="126">
         <v>2</v>
       </c>
-      <c r="AC53" s="90"/>
+      <c r="AC53" s="126"/>
       <c r="AD53" s="33"/>
       <c r="AE53" s="33"/>
       <c r="AF53" s="33"/>
@@ -10323,10 +10323,10 @@
       <c r="BI53" s="27"/>
     </row>
     <row r="54" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A54" s="91" t="s">
+      <c r="A54" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B54" s="91"/>
+      <c r="B54" s="124"/>
       <c r="C54" s="18"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -10352,10 +10352,10 @@
       <c r="Y54" s="33"/>
       <c r="Z54" s="33"/>
       <c r="AA54" s="33"/>
-      <c r="AB54" s="90">
-        <v>1</v>
-      </c>
-      <c r="AC54" s="90"/>
+      <c r="AB54" s="126">
+        <v>1</v>
+      </c>
+      <c r="AC54" s="126"/>
       <c r="AD54" s="33"/>
       <c r="AE54" s="33"/>
       <c r="AF54" s="33"/>
@@ -10390,10 +10390,10 @@
       <c r="BI54" s="27"/>
     </row>
     <row r="55" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A55" s="91" t="s">
+      <c r="A55" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="91"/>
+      <c r="B55" s="124"/>
       <c r="C55" s="18"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -10419,10 +10419,10 @@
       <c r="Y55" s="33"/>
       <c r="Z55" s="33"/>
       <c r="AA55" s="33"/>
-      <c r="AB55" s="90">
-        <v>1</v>
-      </c>
-      <c r="AC55" s="90"/>
+      <c r="AB55" s="126">
+        <v>1</v>
+      </c>
+      <c r="AC55" s="126"/>
       <c r="AD55" s="33"/>
       <c r="AE55" s="33"/>
       <c r="AF55" s="33"/>
@@ -10457,10 +10457,10 @@
       <c r="BI55" s="27"/>
     </row>
     <row r="56" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A56" s="91" t="s">
+      <c r="A56" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="91"/>
+      <c r="B56" s="124"/>
       <c r="C56" s="18"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -10484,10 +10484,10 @@
       <c r="W56" s="33"/>
       <c r="X56" s="33"/>
       <c r="Y56" s="33"/>
-      <c r="Z56" s="90">
+      <c r="Z56" s="126">
         <v>2</v>
       </c>
-      <c r="AA56" s="90"/>
+      <c r="AA56" s="126"/>
       <c r="AB56" s="33"/>
       <c r="AC56" s="33"/>
       <c r="AD56" s="33"/>
@@ -10524,10 +10524,10 @@
       <c r="BI56" s="27"/>
     </row>
     <row r="57" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="91" t="s">
+      <c r="A57" s="124" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="91"/>
+      <c r="B57" s="124"/>
       <c r="C57" s="18"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -10551,10 +10551,10 @@
       <c r="W57" s="33"/>
       <c r="X57" s="33"/>
       <c r="Y57" s="33"/>
-      <c r="Z57" s="90">
+      <c r="Z57" s="126">
         <v>2</v>
       </c>
-      <c r="AA57" s="90"/>
+      <c r="AA57" s="126"/>
       <c r="AB57" s="33"/>
       <c r="AC57" s="33"/>
       <c r="AD57" s="33"/>
@@ -10591,10 +10591,10 @@
       <c r="BI57" s="27"/>
     </row>
     <row r="58" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A58" s="91" t="s">
+      <c r="A58" s="124" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="91"/>
+      <c r="B58" s="124"/>
       <c r="C58" s="18"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -10622,10 +10622,10 @@
       <c r="AA58" s="33"/>
       <c r="AB58" s="33"/>
       <c r="AC58" s="33"/>
-      <c r="AD58" s="90">
-        <v>1</v>
-      </c>
-      <c r="AE58" s="90"/>
+      <c r="AD58" s="126">
+        <v>1</v>
+      </c>
+      <c r="AE58" s="126"/>
       <c r="AF58" s="33"/>
       <c r="AG58" s="33"/>
       <c r="AH58" s="33"/>
@@ -10658,10 +10658,10 @@
       <c r="BI58" s="27"/>
     </row>
     <row r="59" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A59" s="91" t="s">
+      <c r="A59" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="91"/>
+      <c r="B59" s="124"/>
       <c r="C59" s="18"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -10691,10 +10691,10 @@
       <c r="AC59" s="33"/>
       <c r="AD59" s="33"/>
       <c r="AE59" s="33"/>
-      <c r="AF59" s="90">
-        <v>1</v>
-      </c>
-      <c r="AG59" s="90"/>
+      <c r="AF59" s="126">
+        <v>1</v>
+      </c>
+      <c r="AG59" s="126"/>
       <c r="AH59" s="33"/>
       <c r="AI59" s="33"/>
       <c r="AJ59" s="33"/>
@@ -10725,10 +10725,10 @@
       <c r="BI59" s="27"/>
     </row>
     <row r="60" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A60" s="91" t="s">
+      <c r="A60" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="91"/>
+      <c r="B60" s="124"/>
       <c r="C60" s="18"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -10760,10 +10760,10 @@
       <c r="AE60" s="33"/>
       <c r="AF60" s="33"/>
       <c r="AG60" s="33"/>
-      <c r="AH60" s="90">
-        <v>1</v>
-      </c>
-      <c r="AI60" s="90"/>
+      <c r="AH60" s="126">
+        <v>1</v>
+      </c>
+      <c r="AI60" s="126"/>
       <c r="AJ60" s="33"/>
       <c r="AK60" s="33"/>
       <c r="AL60" s="33"/>
@@ -10792,10 +10792,10 @@
       <c r="BI60" s="27"/>
     </row>
     <row r="61" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A61" s="91" t="s">
+      <c r="A61" s="124" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="91"/>
+      <c r="B61" s="124"/>
       <c r="C61" s="18"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -10831,10 +10831,10 @@
       <c r="AI61" s="33"/>
       <c r="AJ61" s="33"/>
       <c r="AK61" s="33"/>
-      <c r="AL61" s="90">
-        <v>1</v>
-      </c>
-      <c r="AM61" s="90"/>
+      <c r="AL61" s="126">
+        <v>1</v>
+      </c>
+      <c r="AM61" s="126"/>
       <c r="AN61" s="33"/>
       <c r="AO61" s="33"/>
       <c r="AP61" s="33"/>
@@ -10859,10 +10859,10 @@
       <c r="BI61" s="27"/>
     </row>
     <row r="62" spans="1:61" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="91" t="s">
+      <c r="A62" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="B62" s="91"/>
+      <c r="B62" s="124"/>
       <c r="C62" s="18"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -10898,10 +10898,10 @@
       <c r="AI62" s="33"/>
       <c r="AJ62" s="33"/>
       <c r="AK62" s="33"/>
-      <c r="AL62" s="90">
-        <v>1</v>
-      </c>
-      <c r="AM62" s="90"/>
+      <c r="AL62" s="126">
+        <v>1</v>
+      </c>
+      <c r="AM62" s="126"/>
       <c r="AN62" s="33"/>
       <c r="AO62" s="33"/>
       <c r="AP62" s="33"/>
@@ -10926,10 +10926,10 @@
       <c r="BI62" s="27"/>
     </row>
     <row r="63" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A63" s="91" t="s">
+      <c r="A63" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="91"/>
+      <c r="B63" s="124"/>
       <c r="C63" s="18"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -10967,10 +10967,10 @@
       <c r="AK63" s="35"/>
       <c r="AL63" s="35"/>
       <c r="AM63" s="35"/>
-      <c r="AN63" s="90">
-        <v>1</v>
-      </c>
-      <c r="AO63" s="90"/>
+      <c r="AN63" s="126">
+        <v>1</v>
+      </c>
+      <c r="AO63" s="126"/>
       <c r="AP63" s="33"/>
       <c r="AQ63" s="33"/>
       <c r="AR63" s="33"/>
@@ -10993,10 +10993,10 @@
       <c r="BI63" s="27"/>
     </row>
     <row r="64" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A64" s="91" t="s">
+      <c r="A64" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="91"/>
+      <c r="B64" s="124"/>
       <c r="C64" s="18"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -11034,10 +11034,10 @@
       <c r="AK64" s="35"/>
       <c r="AL64" s="35"/>
       <c r="AM64" s="35"/>
-      <c r="AN64" s="90">
-        <v>1</v>
-      </c>
-      <c r="AO64" s="90"/>
+      <c r="AN64" s="126">
+        <v>1</v>
+      </c>
+      <c r="AO64" s="126"/>
       <c r="AP64" s="33"/>
       <c r="AQ64" s="33"/>
       <c r="AR64" s="33"/>
@@ -11060,10 +11060,10 @@
       <c r="BI64" s="27"/>
     </row>
     <row r="65" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A65" s="91" t="s">
+      <c r="A65" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="91"/>
+      <c r="B65" s="124"/>
       <c r="C65" s="18"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -11103,10 +11103,10 @@
       <c r="AM65" s="35"/>
       <c r="AN65" s="33"/>
       <c r="AO65" s="33"/>
-      <c r="AP65" s="90">
-        <v>1</v>
-      </c>
-      <c r="AQ65" s="90"/>
+      <c r="AP65" s="126">
+        <v>1</v>
+      </c>
+      <c r="AQ65" s="126"/>
       <c r="AR65" s="33"/>
       <c r="AS65" s="33"/>
       <c r="AT65" s="33"/>
@@ -11127,10 +11127,10 @@
       <c r="BI65" s="27"/>
     </row>
     <row r="66" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A66" s="91" t="s">
+      <c r="A66" s="124" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="91"/>
+      <c r="B66" s="124"/>
       <c r="C66" s="18"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -11170,10 +11170,10 @@
       <c r="AM66" s="35"/>
       <c r="AN66" s="33"/>
       <c r="AO66" s="33"/>
-      <c r="AP66" s="90">
-        <v>1</v>
-      </c>
-      <c r="AQ66" s="90"/>
+      <c r="AP66" s="126">
+        <v>1</v>
+      </c>
+      <c r="AQ66" s="126"/>
       <c r="AR66" s="33"/>
       <c r="AS66" s="33"/>
       <c r="AT66" s="33"/>
@@ -11194,10 +11194,10 @@
       <c r="BI66" s="27"/>
     </row>
     <row r="67" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A67" s="91" t="s">
+      <c r="A67" s="124" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="91"/>
+      <c r="B67" s="124"/>
       <c r="C67" s="18"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -11241,10 +11241,10 @@
       <c r="AQ67" s="33"/>
       <c r="AR67" s="33"/>
       <c r="AS67" s="33"/>
-      <c r="AT67" s="90">
+      <c r="AT67" s="126">
         <v>3</v>
       </c>
-      <c r="AU67" s="90"/>
+      <c r="AU67" s="126"/>
       <c r="AV67" s="33"/>
       <c r="AW67" s="33"/>
       <c r="AX67" s="33"/>
@@ -11261,10 +11261,10 @@
       <c r="BI67" s="27"/>
     </row>
     <row r="68" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A68" s="91" t="s">
+      <c r="A68" s="124" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="91"/>
+      <c r="B68" s="124"/>
       <c r="C68" s="18"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -11308,10 +11308,10 @@
       <c r="AQ68" s="33"/>
       <c r="AR68" s="33"/>
       <c r="AS68" s="33"/>
-      <c r="AT68" s="90">
+      <c r="AT68" s="126">
         <v>2</v>
       </c>
-      <c r="AU68" s="90"/>
+      <c r="AU68" s="126"/>
       <c r="AV68" s="33"/>
       <c r="AW68" s="33"/>
       <c r="AX68" s="33"/>
@@ -11328,10 +11328,10 @@
       <c r="BI68" s="27"/>
     </row>
     <row r="69" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A69" s="91" t="s">
+      <c r="A69" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="91"/>
+      <c r="B69" s="124"/>
       <c r="C69" s="18"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -11379,10 +11379,10 @@
       <c r="AU69" s="33"/>
       <c r="AV69" s="33"/>
       <c r="AW69" s="33"/>
-      <c r="AX69" s="90">
+      <c r="AX69" s="126">
         <v>2</v>
       </c>
-      <c r="AY69" s="90"/>
+      <c r="AY69" s="126"/>
       <c r="AZ69" s="33"/>
       <c r="BA69" s="33"/>
       <c r="BB69" s="33"/>
@@ -11395,10 +11395,10 @@
       <c r="BI69" s="27"/>
     </row>
     <row r="70" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A70" s="91" t="s">
+      <c r="A70" s="124" t="s">
         <v>82</v>
       </c>
-      <c r="B70" s="91"/>
+      <c r="B70" s="124"/>
       <c r="C70" s="18"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -11446,10 +11446,10 @@
       <c r="AU70" s="33"/>
       <c r="AV70" s="33"/>
       <c r="AW70" s="33"/>
-      <c r="AX70" s="90">
+      <c r="AX70" s="126">
         <v>2</v>
       </c>
-      <c r="AY70" s="90"/>
+      <c r="AY70" s="126"/>
       <c r="AZ70" s="33"/>
       <c r="BA70" s="33"/>
       <c r="BB70" s="33"/>
@@ -11462,10 +11462,10 @@
       <c r="BI70" s="27"/>
     </row>
     <row r="71" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A71" s="91" t="s">
+      <c r="A71" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="91"/>
+      <c r="B71" s="124"/>
       <c r="C71" s="18"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -11513,10 +11513,10 @@
       <c r="AU71" s="33"/>
       <c r="AV71" s="33"/>
       <c r="AW71" s="33"/>
-      <c r="AX71" s="90">
+      <c r="AX71" s="126">
         <v>2</v>
       </c>
-      <c r="AY71" s="90"/>
+      <c r="AY71" s="126"/>
       <c r="AZ71" s="33"/>
       <c r="BA71" s="33"/>
       <c r="BB71" s="33"/>
@@ -11529,10 +11529,10 @@
       <c r="BI71" s="27"/>
     </row>
     <row r="72" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A72" s="91" t="s">
+      <c r="A72" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="91"/>
+      <c r="B72" s="124"/>
       <c r="C72" s="18"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -11580,10 +11580,10 @@
       <c r="AU72" s="33"/>
       <c r="AV72" s="33"/>
       <c r="AW72" s="33"/>
-      <c r="AX72" s="90">
+      <c r="AX72" s="126">
         <v>2</v>
       </c>
-      <c r="AY72" s="90"/>
+      <c r="AY72" s="126"/>
       <c r="AZ72" s="33"/>
       <c r="BA72" s="33"/>
       <c r="BB72" s="33"/>
@@ -11596,10 +11596,10 @@
       <c r="BI72" s="27"/>
     </row>
     <row r="73" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="91" t="s">
+      <c r="A73" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="91"/>
+      <c r="B73" s="124"/>
       <c r="C73" s="18"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -11645,10 +11645,10 @@
       <c r="AS73" s="33"/>
       <c r="AT73" s="33"/>
       <c r="AU73" s="33"/>
-      <c r="AV73" s="90" t="s">
-        <v>167</v>
-      </c>
-      <c r="AW73" s="90"/>
+      <c r="AV73" s="126" t="s">
+        <v>166</v>
+      </c>
+      <c r="AW73" s="126"/>
       <c r="AX73" s="33"/>
       <c r="AY73" s="33"/>
       <c r="AZ73" s="33"/>
@@ -11663,10 +11663,10 @@
       <c r="BI73" s="27"/>
     </row>
     <row r="74" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A74" s="91" t="s">
+      <c r="A74" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="B74" s="91"/>
+      <c r="B74" s="124"/>
       <c r="C74" s="18"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -11712,8 +11712,8 @@
       <c r="AS74" s="33"/>
       <c r="AT74" s="33"/>
       <c r="AU74" s="33"/>
-      <c r="AV74" s="90"/>
-      <c r="AW74" s="90"/>
+      <c r="AV74" s="126"/>
+      <c r="AW74" s="126"/>
       <c r="AX74" s="33"/>
       <c r="AY74" s="33"/>
       <c r="AZ74" s="33"/>
@@ -11728,10 +11728,10 @@
       <c r="BI74" s="27"/>
     </row>
     <row r="75" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A75" s="91" t="s">
+      <c r="A75" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="91"/>
+      <c r="B75" s="124"/>
       <c r="C75" s="18"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -11777,8 +11777,8 @@
       <c r="AS75" s="33"/>
       <c r="AT75" s="33"/>
       <c r="AU75" s="33"/>
-      <c r="AV75" s="90"/>
-      <c r="AW75" s="90"/>
+      <c r="AV75" s="126"/>
+      <c r="AW75" s="126"/>
       <c r="AX75" s="33"/>
       <c r="AY75" s="33"/>
       <c r="AZ75" s="33"/>
@@ -11793,10 +11793,10 @@
       <c r="BI75" s="27"/>
     </row>
     <row r="76" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="91" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" s="91"/>
+      <c r="A76" s="124" t="s">
+        <v>172</v>
+      </c>
+      <c r="B76" s="124"/>
       <c r="C76" s="18"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -11842,8 +11842,8 @@
       <c r="AS76" s="33"/>
       <c r="AT76" s="33"/>
       <c r="AU76" s="33"/>
-      <c r="AV76" s="90"/>
-      <c r="AW76" s="90"/>
+      <c r="AV76" s="126"/>
+      <c r="AW76" s="126"/>
       <c r="AX76" s="33"/>
       <c r="AY76" s="33"/>
       <c r="AZ76" s="33"/>
@@ -11858,10 +11858,10 @@
       <c r="BI76" s="27"/>
     </row>
     <row r="77" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A77" s="91" t="s">
-        <v>168</v>
-      </c>
-      <c r="B77" s="91"/>
+      <c r="A77" s="124" t="s">
+        <v>167</v>
+      </c>
+      <c r="B77" s="124"/>
       <c r="C77" s="18"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -11907,8 +11907,8 @@
       <c r="AS77" s="33"/>
       <c r="AT77" s="33"/>
       <c r="AU77" s="33"/>
-      <c r="AV77" s="90"/>
-      <c r="AW77" s="90"/>
+      <c r="AV77" s="126"/>
+      <c r="AW77" s="126"/>
       <c r="AX77" s="33"/>
       <c r="AY77" s="33"/>
       <c r="AZ77" s="33"/>
@@ -11923,10 +11923,10 @@
       <c r="BI77" s="27"/>
     </row>
     <row r="78" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="B78" s="91"/>
+      <c r="A78" s="124" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" s="124"/>
       <c r="C78" s="18"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -11972,8 +11972,8 @@
       <c r="AS78" s="33"/>
       <c r="AT78" s="33"/>
       <c r="AU78" s="33"/>
-      <c r="AV78" s="90"/>
-      <c r="AW78" s="90"/>
+      <c r="AV78" s="126"/>
+      <c r="AW78" s="126"/>
       <c r="AX78" s="33"/>
       <c r="AY78" s="33"/>
       <c r="AZ78" s="33"/>
@@ -12052,7 +12052,7 @@
     </row>
     <row r="80" spans="1:61" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B80" s="44"/>
       <c r="C80" s="44"/>
@@ -12116,13 +12116,13 @@
       <c r="BI80" s="27"/>
     </row>
     <row r="81" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="106" t="s">
-        <v>171</v>
-      </c>
-      <c r="B81" s="107" t="s">
-        <v>162</v>
-      </c>
-      <c r="C81" s="108"/>
+      <c r="A81" s="91" t="s">
+        <v>170</v>
+      </c>
+      <c r="B81" s="92" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" s="93"/>
       <c r="D81" s="44"/>
       <c r="E81" s="44"/>
       <c r="F81" s="44"/>
@@ -12183,16 +12183,16 @@
       <c r="BI81" s="27"/>
     </row>
     <row r="82" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A82" s="110" t="s">
+      <c r="A82" s="118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="B82" s="102" t="s">
+      <c r="C82" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="C82" s="96" t="s">
-        <v>121</v>
-      </c>
-      <c r="D82" s="105"/>
+      <c r="D82" s="90"/>
       <c r="E82" s="44"/>
       <c r="F82" s="44"/>
       <c r="G82" s="44"/>
@@ -12252,14 +12252,14 @@
       <c r="BI82" s="27"/>
     </row>
     <row r="83" spans="1:61" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="111"/>
-      <c r="B83" s="104">
+      <c r="A83" s="121"/>
+      <c r="B83" s="89">
         <v>2170</v>
       </c>
-      <c r="C83" s="97">
+      <c r="C83" s="84">
         <v>2590</v>
       </c>
-      <c r="D83" s="105"/>
+      <c r="D83" s="90"/>
       <c r="E83" s="44"/>
       <c r="F83" s="44"/>
       <c r="G83" s="44"/>
@@ -12319,16 +12319,16 @@
       <c r="BI83" s="27"/>
     </row>
     <row r="84" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A84" s="109" t="s">
-        <v>118</v>
+      <c r="A84" s="120" t="s">
+        <v>117</v>
       </c>
       <c r="B84" s="72">
         <v>10</v>
       </c>
-      <c r="C84" s="98">
+      <c r="C84" s="85">
         <v>11</v>
       </c>
-      <c r="D84" s="94"/>
+      <c r="D84" s="81"/>
       <c r="E84" s="44"/>
       <c r="F84" s="44"/>
       <c r="G84" s="44"/>
@@ -12388,14 +12388,14 @@
       <c r="BI84" s="27"/>
     </row>
     <row r="85" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A85" s="103"/>
-      <c r="B85" s="104">
+      <c r="A85" s="114"/>
+      <c r="B85" s="89">
         <v>34</v>
       </c>
-      <c r="C85" s="97">
+      <c r="C85" s="84">
         <v>34</v>
       </c>
-      <c r="D85" s="95"/>
+      <c r="D85" s="82"/>
       <c r="E85" s="44"/>
       <c r="F85" s="44"/>
       <c r="G85" s="44"/>
@@ -12455,16 +12455,16 @@
       <c r="BI85" s="27"/>
     </row>
     <row r="86" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A86" s="101" t="s">
-        <v>172</v>
-      </c>
-      <c r="B86" s="102">
+      <c r="A86" s="113" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" s="88">
         <v>10</v>
       </c>
-      <c r="C86" s="96">
+      <c r="C86" s="83">
         <v>11</v>
       </c>
-      <c r="D86" s="94"/>
+      <c r="D86" s="81"/>
       <c r="E86" s="44"/>
       <c r="F86" s="44"/>
       <c r="G86" s="44"/>
@@ -12524,14 +12524,14 @@
       <c r="BI86" s="27"/>
     </row>
     <row r="87" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A87" s="103"/>
-      <c r="B87" s="104">
+      <c r="A87" s="114"/>
+      <c r="B87" s="89">
         <v>34</v>
       </c>
-      <c r="C87" s="97">
+      <c r="C87" s="84">
         <v>33</v>
       </c>
-      <c r="D87" s="95"/>
+      <c r="D87" s="82"/>
       <c r="E87" s="44"/>
       <c r="F87" s="44"/>
       <c r="G87" s="44"/>
@@ -12592,12 +12592,12 @@
     </row>
     <row r="88" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A88" s="80" t="s">
+        <v>163</v>
+      </c>
+      <c r="B88" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="B88" s="99" t="s">
-        <v>165</v>
-      </c>
-      <c r="C88" s="100"/>
+      <c r="C88" s="87"/>
       <c r="D88" s="27"/>
       <c r="E88" s="44"/>
       <c r="F88" s="44"/>
@@ -12722,7 +12722,7 @@
     </row>
     <row r="90" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A90" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B90" s="27"/>
       <c r="C90" s="27"/>
@@ -12787,7 +12787,7 @@
     </row>
     <row r="91" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A91" s="50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B91" s="27"/>
       <c r="C91" s="27"/>
@@ -12852,7 +12852,7 @@
     </row>
     <row r="92" spans="1:61" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B92" s="27"/>
       <c r="C92" s="27"/>
@@ -12917,7 +12917,7 @@
     </row>
     <row r="93" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A93" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B93" s="27"/>
       <c r="C93" s="27"/>
@@ -12982,6 +12982,139 @@
     </row>
   </sheetData>
   <mergeCells count="157">
+    <mergeCell ref="P12:Q13"/>
+    <mergeCell ref="R12:S13"/>
+    <mergeCell ref="AV12:AW13"/>
+    <mergeCell ref="T12:U13"/>
+    <mergeCell ref="V12:W13"/>
+    <mergeCell ref="X12:Y13"/>
+    <mergeCell ref="Z12:AA13"/>
+    <mergeCell ref="BD12:BE13"/>
+    <mergeCell ref="BF12:BG13"/>
+    <mergeCell ref="AL12:AM13"/>
+    <mergeCell ref="AP12:AQ13"/>
+    <mergeCell ref="AR12:AS13"/>
+    <mergeCell ref="AT12:AU13"/>
+    <mergeCell ref="AB12:AC13"/>
+    <mergeCell ref="AD12:AE13"/>
+    <mergeCell ref="AF12:AG13"/>
+    <mergeCell ref="AH12:AI13"/>
+    <mergeCell ref="AJ12:AK13"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AX12:AY13"/>
+    <mergeCell ref="BB12:BC13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="J12:K13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="N12:O13"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="Z42:AA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="Z43:AA43"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="V38:W38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="X40:Y40"/>
+    <mergeCell ref="BD47:BE47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="BD48:BE48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="BF49:BG49"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="AZ44:BA44"/>
+    <mergeCell ref="BB44:BC44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="AZ45:BA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="BB46:BC46"/>
+    <mergeCell ref="BF50:BG50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="AD51:AE51"/>
+    <mergeCell ref="AF51:AG51"/>
+    <mergeCell ref="AH51:AI51"/>
+    <mergeCell ref="AJ51:AK51"/>
+    <mergeCell ref="AL51:AM51"/>
+    <mergeCell ref="AN51:AO51"/>
+    <mergeCell ref="AP51:AQ51"/>
+    <mergeCell ref="AB54:AC54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="AB55:AC55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="Z56:AA56"/>
+    <mergeCell ref="AR51:AS51"/>
+    <mergeCell ref="AT51:AU51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="AJ52:AK52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="AB53:AC53"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="AP65:AQ65"/>
+    <mergeCell ref="AH60:AI60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="AL61:AM61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="AL62:AM62"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="Z57:AA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="AD58:AE58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="AF59:AG59"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="AX72:AY72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="AV73:AW78"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="AX69:AY69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="AX70:AY70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="AX71:AY71"/>
+    <mergeCell ref="AP66:AQ66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="AT67:AU67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="AT68:AU68"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="AN63:AO63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="AN64:AO64"/>
     <mergeCell ref="A84:A85"/>
     <mergeCell ref="A82:A83"/>
     <mergeCell ref="A86:A87"/>
@@ -13006,139 +13139,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="AX72:AY72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="AV73:AW78"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="AX69:AY69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="AX70:AY70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="AX71:AY71"/>
-    <mergeCell ref="AP66:AQ66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="AT67:AU67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="AT68:AU68"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="AN63:AO63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="AN64:AO64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="AP65:AQ65"/>
-    <mergeCell ref="AH60:AI60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="AL61:AM61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="AL62:AM62"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="Z57:AA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="AD58:AE58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="AF59:AG59"/>
-    <mergeCell ref="AB54:AC54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="AB55:AC55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="Z56:AA56"/>
-    <mergeCell ref="AR51:AS51"/>
-    <mergeCell ref="AT51:AU51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="AJ52:AK52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="AB53:AC53"/>
-    <mergeCell ref="BF50:BG50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="AD51:AE51"/>
-    <mergeCell ref="AF51:AG51"/>
-    <mergeCell ref="AH51:AI51"/>
-    <mergeCell ref="AJ51:AK51"/>
-    <mergeCell ref="AL51:AM51"/>
-    <mergeCell ref="AN51:AO51"/>
-    <mergeCell ref="AP51:AQ51"/>
-    <mergeCell ref="BD47:BE47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="BD48:BE48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="BF49:BG49"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="AZ44:BA44"/>
-    <mergeCell ref="BB44:BC44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="AZ45:BA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="BB46:BC46"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="Z42:AA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="Z43:AA43"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="V38:W38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="X40:Y40"/>
-    <mergeCell ref="R35:S35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="R34:S34"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AX12:AY13"/>
-    <mergeCell ref="BB12:BC13"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="J12:K13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="N12:O13"/>
-    <mergeCell ref="P12:Q13"/>
-    <mergeCell ref="R12:S13"/>
-    <mergeCell ref="AV12:AW13"/>
-    <mergeCell ref="T12:U13"/>
-    <mergeCell ref="V12:W13"/>
-    <mergeCell ref="X12:Y13"/>
-    <mergeCell ref="Z12:AA13"/>
-    <mergeCell ref="BD12:BE13"/>
-    <mergeCell ref="BF12:BG13"/>
-    <mergeCell ref="AL12:AM13"/>
-    <mergeCell ref="AP12:AQ13"/>
-    <mergeCell ref="AR12:AS13"/>
-    <mergeCell ref="AT12:AU13"/>
-    <mergeCell ref="AB12:AC13"/>
-    <mergeCell ref="AD12:AE13"/>
-    <mergeCell ref="AF12:AG13"/>
-    <mergeCell ref="AH12:AI13"/>
-    <mergeCell ref="AJ12:AK13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>